<commit_message>
feat: alteração no checklist, e criação/edição do artefato Visão
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/Checklist Verificacao de Projeto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12E16D3-8AD5-4F70-887F-6B698B454198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE48C2E-95E6-48C6-8283-085F14C93C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8402,8 +8402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -10463,17 +10463,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -11242,11 +11242,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:F1"/>
@@ -11254,6 +11249,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28" xr:uid="{00000000-0002-0000-0400-000000000000}">

</xml_diff>

<commit_message>
feat: pequenos ajustes em história do usuário, checklist e planejamento e controle do projeto.
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/Checklist Verificacao de Projeto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE48C2E-95E6-48C6-8283-085F14C93C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB7B310-DF00-49FD-AB24-D9EC5F81569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="117">
   <si>
     <t>Ambiente</t>
   </si>
@@ -944,9 +944,6 @@
     <t>Os casos de uso e atores possuem descrições claras e objetivas de forma a não necessitar que alguém explique-o verbalmente?</t>
   </si>
   <si>
-    <t>Se criados, as especificações para os casos de uso/histórias de usuário são testáveis, ou seja, é possível identificar as entradas e verificar se as saída estão corretas?</t>
-  </si>
-  <si>
     <t>Foi criado/atualizado o modelo de negócio das entidades? (diagrama de classes)</t>
   </si>
   <si>
@@ -1047,6 +1044,15 @@
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>Parcialmente</t>
+  </si>
+  <si>
+    <t>Se criados, as especificações para os casos de uso/histórias de usuário são testáveis, ou seja, é possível identificar as entradas e verificar se as saídas estão corretas?</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1602,7 +1608,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.95833333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1840,13 +1846,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1858,10 +1864,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1974,7 +1980,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2173,13 +2179,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2188,7 +2194,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2197,7 +2203,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -7318,7 +7324,7 @@
       </c>
       <c r="B3" s="20">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>1</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7382,55 +7388,55 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
       <c r="N1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" t="s">
         <v>92</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>93</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>95</v>
-      </c>
-      <c r="R1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="e">
+      <c r="B2" s="25">
         <f>('Ver-Iniciação1'!$G$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="C2" s="25">
         <f>('Ver-Iniciação1'!$H$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="D2" s="25">
         <f>('Ver-Iniciação1'!$I$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E2" s="25">
         <f>('Ver-Iniciação1'!$J$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>2</v>
@@ -7496,21 +7502,21 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="e">
+      <c r="B4" s="25">
         <f>('Ver-Iniciação1'!$G$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C4" s="25" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="25">
         <f>('Ver-Iniciação1'!$H$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="D4" s="25">
         <f>('Ver-Iniciação1'!$I$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E4" s="25">
         <f>('Ver-Iniciação1'!$J$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>#DIV/0!</v>
+        <v>0.2</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -7536,21 +7542,21 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="25" t="e">
+      <c r="B5" s="25">
         <f>('Ver-Iniciação1'!$G$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25">
         <f>('Ver-Iniciação1'!$H$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25">
         <f>('Ver-Iniciação1'!$I$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25">
         <f>('Ver-Iniciação1'!$J$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="N5" t="s">
         <v>4</v>
@@ -7576,21 +7582,21 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="e">
+      <c r="B6" s="25">
         <f>('Ver-Iniciação1'!$G$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="C6" s="25">
         <f>('Ver-Iniciação1'!$H$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="D6" s="25">
         <f>('Ver-Iniciação1'!$I$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
         <f>('Ver-Iniciação1'!$J$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="N6" t="s">
         <v>36</v>
@@ -7616,21 +7622,21 @@
       <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="25" t="e">
+      <c r="B7" s="25">
         <f>('Ver-Iniciação1'!$G$25/SUM('Ver-Iniciação1'!$G$25:'Ver-Iniciação1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="C7" s="25">
         <f>('Ver-Iniciação1'!$H$25/SUM('Ver-Iniciação1'!$G$25:'Ver-Iniciação1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="D7" s="25">
         <f>('Ver-Iniciação1'!$I$25/SUM('Ver-Iniciação1'!$G$25:'Ver-Iniciação1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
         <f>('Ver-Iniciação1'!$J$25/SUM('Ver-Iniciação1'!$G$25:'Ver-Iniciação1'!$J$25))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="N7" t="s">
         <v>5</v>
@@ -7694,7 +7700,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="25" t="e">
         <f>('Ver-Iniciação1'!#REF!/SUM('Ver-Iniciação1'!#REF!:'Ver-Iniciação1'!#REF!))</f>
@@ -7736,21 +7742,21 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="25" t="e">
+      <c r="B10" s="25">
         <f>('Ver-Iniciação1'!$G$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="25" t="e">
+        <v>0.875</v>
+      </c>
+      <c r="C10" s="25">
         <f>('Ver-Iniciação1'!$H$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="D10" s="25">
         <f>('Ver-Iniciação1'!$I$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E10" s="25">
         <f>('Ver-Iniciação1'!$J$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>#DIV/0!</v>
+        <v>0.125</v>
       </c>
       <c r="N10" t="s">
         <v>13</v>
@@ -7776,21 +7782,21 @@
       <c r="A11" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="25" t="e">
+      <c r="B11" s="25">
         <f>('Ver-Iniciação1'!$G$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="25" t="e">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="25">
         <f>('Ver-Iniciação1'!$H$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="25" t="e">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="25">
         <f>('Ver-Iniciação1'!$I$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E11" s="25">
         <f>('Ver-Iniciação1'!$J$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="N11" t="s">
         <v>56</v>
@@ -7854,19 +7860,19 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
         <v>92</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>94</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>95</v>
-      </c>
-      <c r="E22" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -7911,19 +7917,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M24" t="s">
+        <v>91</v>
+      </c>
+      <c r="N24" t="s">
         <v>92</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>93</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>94</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>95</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -8402,8 +8408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8442,7 +8448,7 @@
       <c r="E2" s="40"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>1</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -8502,7 +8508,7 @@
       </c>
       <c r="J5">
         <f>COUNTIF(D6,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
@@ -8513,7 +8519,9 @@
       <c r="C6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
@@ -8530,7 +8538,7 @@
       <c r="F7" s="12"/>
       <c r="G7">
         <f>COUNTIF(D8:D12,"Sim")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <f>COUNTIF(D8:D12,"Parcialmente")</f>
@@ -8554,7 +8562,7 @@
         <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -8568,7 +8576,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -8581,7 +8589,9 @@
       <c r="C10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
@@ -8593,7 +8603,9 @@
       <c r="C11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -8605,7 +8617,9 @@
       <c r="C12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -8620,7 +8634,7 @@
       <c r="F13" s="12"/>
       <c r="G13">
         <f>COUNTIF(D14:D18,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <f>COUNTIF(D14:D18,"Parcialmente")</f>
@@ -8632,7 +8646,7 @@
       </c>
       <c r="J13">
         <f>COUNTIF(D14:D18,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15">
@@ -8643,7 +8657,9 @@
       <c r="C14" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
@@ -8655,7 +8671,9 @@
       <c r="C15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
@@ -8667,7 +8685,9 @@
       <c r="C16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
@@ -8679,7 +8699,9 @@
       <c r="C17" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
@@ -8691,7 +8713,9 @@
       <c r="C18" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
@@ -8699,14 +8723,14 @@
       <c r="A19" s="31"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19">
         <f>COUNTIF(D20:D21,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <f>COUNTIF(D20:D21,"Parcialmente")</f>
@@ -8729,7 +8753,9 @@
       <c r="C20" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -8739,9 +8765,11 @@
         <v>13</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -8756,7 +8784,7 @@
       <c r="F22" s="12"/>
       <c r="G22">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
@@ -8779,7 +8807,9 @@
       <c r="C23" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
@@ -8791,7 +8821,9 @@
       <c r="C24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
@@ -8818,7 +8850,7 @@
       </c>
       <c r="J25">
         <f>COUNTIF(D26:D27,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15">
@@ -8829,7 +8861,9 @@
       <c r="C26" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
@@ -8841,7 +8875,9 @@
       <c r="C27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -8856,7 +8892,7 @@
       <c r="F28" s="12"/>
       <c r="G28">
         <f>COUNTIF(D29:D36,"Sim")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H28">
         <f>COUNTIF(D29:D36,"Parcialmente")</f>
@@ -8868,7 +8904,7 @@
       </c>
       <c r="J28">
         <f>COUNTIF(D29:D36,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15">
@@ -8879,7 +8915,9 @@
       <c r="C29" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
@@ -8891,7 +8929,9 @@
       <c r="C30" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
@@ -8901,9 +8941,11 @@
         <v>23</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -8913,9 +8955,11 @@
         <v>24</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
@@ -8925,9 +8969,11 @@
         <v>25</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -8937,9 +8983,11 @@
         <v>26</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="18.75" customHeight="1">
@@ -8948,9 +8996,11 @@
         <v>27</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
@@ -8960,9 +9010,11 @@
         <v>28</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
@@ -8979,11 +9031,11 @@
       <c r="F37" s="12"/>
       <c r="G37">
         <f>COUNTIF(D38:D41,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37">
         <f>COUNTIF(D38:D41,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <f>COUNTIF(D38:D41,"Não")</f>
@@ -9002,7 +9054,9 @@
       <c r="C38" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -9014,7 +9068,9 @@
       <c r="C39" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
@@ -9026,7 +9082,9 @@
       <c r="C40" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
@@ -9038,7 +9096,9 @@
       <c r="C41" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
@@ -9159,7 +9219,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="8"/>
@@ -9197,7 +9257,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="8"/>
@@ -9225,7 +9285,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="8"/>
@@ -9239,7 +9299,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -9251,7 +9311,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="8"/>
@@ -9279,7 +9339,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="8"/>
@@ -9481,7 +9541,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="8"/>
@@ -9493,7 +9553,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="8"/>
@@ -9505,7 +9565,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="8"/>
@@ -9529,7 +9589,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="8"/>
@@ -9557,7 +9617,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="8"/>
@@ -9581,7 +9641,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="8"/>
@@ -9691,7 +9751,7 @@
         <v>32</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="8"/>
@@ -9719,7 +9779,7 @@
         <v>33</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="8"/>
@@ -9845,7 +9905,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="8"/>
@@ -9883,7 +9943,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="8"/>
@@ -9909,7 +9969,7 @@
       <c r="A9" s="31"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -9921,7 +9981,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="8"/>
@@ -9949,7 +10009,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="8"/>
@@ -10063,7 +10123,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="8"/>
@@ -10103,7 +10163,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="8"/>
@@ -10115,7 +10175,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="8"/>
@@ -10127,7 +10187,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="8"/>
@@ -10215,7 +10275,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="8"/>
@@ -10239,7 +10299,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="8"/>
@@ -10267,7 +10327,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="8"/>
@@ -10377,7 +10437,7 @@
       <c r="A39" s="30"/>
       <c r="B39" s="5"/>
       <c r="C39" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="8"/>
@@ -10399,7 +10459,7 @@
         <v>33</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="8"/>
@@ -10427,7 +10487,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="8"/>
@@ -10582,7 +10642,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="8"/>
@@ -10620,7 +10680,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="8"/>
@@ -10658,7 +10718,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="8"/>
@@ -10686,7 +10746,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="8"/>
@@ -10840,7 +10900,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="8"/>
@@ -10876,7 +10936,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="8"/>
@@ -10904,7 +10964,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="8"/>
@@ -11018,7 +11078,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="8"/>
@@ -11046,7 +11106,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="8"/>
@@ -11070,7 +11130,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="8"/>
@@ -11156,7 +11216,7 @@
       <c r="A40" s="30"/>
       <c r="B40" s="5"/>
       <c r="C40" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="8"/>
@@ -11178,7 +11238,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="8"/>
@@ -11206,7 +11266,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="8"/>

</xml_diff>